<commit_message>
Incorporated filter options and NLP
Incorporated:
- Filtering options: Type, Serving Size, Decaf Coffee?, Coffee Select, Technique Selector (TF-IDF, BoW)
- Coffee Information,
- TF-IDF Recommendation
- Bag of Words Recommendation
- Word Cloud
- Taste Profile visualization
- Feature Results (TF-IDF/Bag of Words)
-
</commit_message>
<xml_diff>
--- a/NespressoTrainingApp/data/CoffeeData.xlsx
+++ b/NespressoTrainingApp/data/CoffeeData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunal\Documents\Nespresso\Version 1\NespressoTrainingApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1876ACB2-4BF4-4B63-91E8-FF8EC2EBC51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0931DD1A-C551-40F2-AEF6-63E8939A549E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="613">
   <si>
     <t>Name</t>
   </si>
@@ -1019,6 +1019,856 @@
   </si>
   <si>
     <t>Balanced, Intense</t>
+  </si>
+  <si>
+    <t>Inspirazione Napoli</t>
+  </si>
+  <si>
+    <t>Kazaar</t>
+  </si>
+  <si>
+    <t>Ristretto</t>
+  </si>
+  <si>
+    <t>Ristretto Decaffeinato</t>
+  </si>
+  <si>
+    <t>Arpeggio</t>
+  </si>
+  <si>
+    <t>Arpeggio Decaffeinato</t>
+  </si>
+  <si>
+    <t>Inspirazione Venezia</t>
+  </si>
+  <si>
+    <t>Inspirazione Roma</t>
+  </si>
+  <si>
+    <t>Livanto</t>
+  </si>
+  <si>
+    <t>OL1</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Dark &amp; Creamy</t>
+  </si>
+  <si>
+    <t>The most intense and darkest roast in this range, inspired by the capital of coffee, reveals the deep-rooted roasting traditions of Naples. Its depth of character should come as no surprise.</t>
+  </si>
+  <si>
+    <t>Ispirazione Napoli pays tribute to the short, strong and dark espressos of this southern Italian coastal city. It’s a velvety, creamy cup with an extremely thick body and a kiss of pleasant bitterness in its aftertaste. A velvety, creamy cup with an extremely thick body and pleasantly bitter cocoa notes.</t>
+  </si>
+  <si>
+    <t>Ristretto 25ml, Espresso 40ml</t>
+  </si>
+  <si>
+    <t>Intense, Roasted</t>
+  </si>
+  <si>
+    <t>57 g</t>
+  </si>
+  <si>
+    <t>Inspirazione Italiana</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16216638324766/ispirazione-napoli-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/ispirazione-napoli_L.png</t>
+  </si>
+  <si>
+    <t>OL2</t>
+  </si>
+  <si>
+    <t>OL3</t>
+  </si>
+  <si>
+    <t>OL4</t>
+  </si>
+  <si>
+    <t>OL5</t>
+  </si>
+  <si>
+    <t>OL6</t>
+  </si>
+  <si>
+    <t>OL7</t>
+  </si>
+  <si>
+    <t>OL8</t>
+  </si>
+  <si>
+    <t>OL9</t>
+  </si>
+  <si>
+    <t>Intense &amp; Syrupy</t>
+  </si>
+  <si>
+    <t>A long, dark roast inspired by the union of Sicilian coffee artistry and African and Arabian heritage is guaranteed to spice things up.</t>
+  </si>
+  <si>
+    <t>You’ll taste the audacious bitterness and peppery notes leaping out through the thick syrupy body. Together the Arabica and Robusta balance each other out in this espresso. It reflects both the Palermo coastal lifestyle and its rich history. You can sit back in the sun and enjoy your Kazaar on the terrace, with everything from the food on your plate to the architecture surrounding you whispering the histories of all who’ve passed through Palermo.</t>
+  </si>
+  <si>
+    <t>Woody, Spicy</t>
+  </si>
+  <si>
+    <t>60 g</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16283547566110/Palermo-kazaar-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/ispirazione-palermo-kazaar_L.png</t>
+  </si>
+  <si>
+    <t>Powerful &amp; Contrasting</t>
+  </si>
+  <si>
+    <t>This medium dark roast embodies Italy’s iconic coffee culture in just a short, quick sip.</t>
+  </si>
+  <si>
+    <t>A roasty and intense coffee but with fruity notes and a hint of acidity dancing through the blend – Ristretto is mysterious and magnetic in its complexity. It’s a profile worthy of an ambassador – a coffee that explains Italians’ passion for coffee and makes sense of why it’s ingrained in daily life. Extracted to the classic 25 ml, you’ll soon see how right the Italians are – this drop of deliciousness shows how less can truly be more.</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16217625559070/ispirazione-ristretto-italiano-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/ispirazione-ristretto_L.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This medium dark roast embodies Italy’s iconic coffee culture in just a short, quick sip.
+</t>
+  </si>
+  <si>
+    <t>Boldly roasty but balanced out by soft cocoa notes. You may catch some of the subtle acidity and fruity notes that make this Nespresso Decaf capsule so mysteriously complex. It’s a profile worthy of an ambassador – a coffee that explains Italians’ passion for coffee and makes sense of why it’s ingrained in daily life. Extracted to the classic 25 ml, you’ll soon see how right the Italians are – this drop of deliciousness shows how less can truly be more.</t>
+  </si>
+  <si>
+    <t>Decaffeinated roast and ground coffee</t>
+  </si>
+  <si>
+    <t>58 g</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16262679461918/ristretto-italiano-decaffeinato-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/ispirazione-ristretto-decaffeinato_XL.png</t>
+  </si>
+  <si>
+    <t>Intense &amp; Creamy</t>
+  </si>
+  <si>
+    <t>A short and dark roasted masterpiece such as this, can only come from the heart. Or in this instance, the cultural and artistic heart of Italy.</t>
+  </si>
+  <si>
+    <t>Arpeggio is dense and creamy with bold roasty and cocoa notes. The crema gives it a creamy, velvety texture that is irresistible. You might even call it high art.</t>
+  </si>
+  <si>
+    <t>Intense, Very Roasted, Cocoa</t>
+  </si>
+  <si>
+    <t>53 g</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15990477783070/firenze-arpeggio-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/ispirazione-firenze-arpeggio_L.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A short and dark-roasted masterpiece such as this can only come from the cultural and artistic heart of Italy.
+</t>
+  </si>
+  <si>
+    <t>Arpeggio Decaffeinato is as dense and creamy as the no decaffeinated version. Decaffeination doesn’t diminish the bold roasty and cocoa notes. The crema gives it a creamy, velvety texture that is irresistible.</t>
+  </si>
+  <si>
+    <t>Very Roasted, Cocoa</t>
+  </si>
+  <si>
+    <t>Very Roasted, Hint of Fruity</t>
+  </si>
+  <si>
+    <t>55 g</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15942162972702/firenze-arpeggio-decaffeinato-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/ispirazione-firenze-arpeggio-decaffeinato_L.png</t>
+  </si>
+  <si>
+    <t>Balanced &amp; Thick Body</t>
+  </si>
+  <si>
+    <t>Unsurprisingly, this long roast wasn’t discovered overnight, but was rather inspired by Italy’s enduring roasting traditions that have been passed down through generations.</t>
+  </si>
+  <si>
+    <t>Ispirazione Venezia is a mellow, rounded and delicately aromatic coffee that will remind you of coffee beans fresh out of the roaster – taking you back in time to the early days of Italy’s coffee trade. Its lighter roast keeps the delicate aromas intensely present while developing a thick body. In Venezia you can’t miss the distinct cereal fragrance and those notes of sweet caramel that we all find so reassuring.</t>
+  </si>
+  <si>
+    <t>Roasted</t>
+  </si>
+  <si>
+    <t>56 g</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441095725086/ispirazione-venezia-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/13953171390494/C-0472-Main-PDP-IspirazioneItaliana-Venezia-OL.jpg?impolicy=productPdpSafeZone&amp;imwidth=1238</t>
+  </si>
+  <si>
+    <t>Full &amp; Balanced</t>
+  </si>
+  <si>
+    <t>Combining the ancient character of Rome with a twist of modernity, this short roast balances intensity with elegant aromatics, reflecting the complexity of this great city. Thankfully, making one for yourself is less complex.</t>
+  </si>
+  <si>
+    <t>From the days of Ancient Rome, a great many cultures passed through this metropolis. Different layers of civilization towering up to the present day when Modern Rome adds its layer of elegance to the rich history of the city. Ispirazione Roma, too, is beautifully complex. There’s a subtle balance between the strength of the roastiness, the depth of the woodsy, cereal notes, and the finesse of the acidity and elegant aromatics.</t>
+  </si>
+  <si>
+    <t>Woody, Cereal</t>
+  </si>
+  <si>
+    <t>50 g</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441097035806/ispirazione-roma-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/ispirazione-roma_L.png</t>
+  </si>
+  <si>
+    <t>Round &amp; Balanced</t>
+  </si>
+  <si>
+    <t>In honour of Genoa, the gateway to the world, we used some of the finest Latin American Arabicas to create this sweet, medium roast.</t>
+  </si>
+  <si>
+    <t>Livanto is a smooth, rounded and delicately aromatic coffee. Its lighter roast develops the smooth and full body and keeps the finer aromas present. You’ll catch a toasted cereal fragrance and sweet caramel notes.</t>
+  </si>
+  <si>
+    <t>Balanced</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441097134110/ispirazione-genova-livanto-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/13245281894430/C-0477-Main-PDP-IspirazioneItaliana-GenovaLivanto-OL.jpg?impolicy=productPdpSafeZone&amp;imwidth=1238</t>
+  </si>
+  <si>
+    <t>OL10</t>
+  </si>
+  <si>
+    <t>Cape Town Lungo</t>
+  </si>
+  <si>
+    <t>Miami Espresso</t>
+  </si>
+  <si>
+    <t>Rio De Janeiro Espresso</t>
+  </si>
+  <si>
+    <t>Instanbul Espresso</t>
+  </si>
+  <si>
+    <t>Stockholm Lungo</t>
+  </si>
+  <si>
+    <t>Paris Espresso</t>
+  </si>
+  <si>
+    <t>Tokyo Lungo</t>
+  </si>
+  <si>
+    <t>Vienna Lungo</t>
+  </si>
+  <si>
+    <t>Shanghai Lungo</t>
+  </si>
+  <si>
+    <t>Buenos Aires Lungo</t>
+  </si>
+  <si>
+    <t>OL11</t>
+  </si>
+  <si>
+    <t>OL12</t>
+  </si>
+  <si>
+    <t>OL13</t>
+  </si>
+  <si>
+    <t>OL14</t>
+  </si>
+  <si>
+    <t>OL15</t>
+  </si>
+  <si>
+    <t>OL16</t>
+  </si>
+  <si>
+    <t>OL17</t>
+  </si>
+  <si>
+    <t>OL18</t>
+  </si>
+  <si>
+    <t>OL19</t>
+  </si>
+  <si>
+    <t>World Explorations</t>
+  </si>
+  <si>
+    <t>Lungo</t>
+  </si>
+  <si>
+    <t>110ml</t>
+  </si>
+  <si>
+    <t>Potent &amp; Roasted</t>
+  </si>
+  <si>
+    <t>A deep-roasted, intense, and full-bodied cup with a woodsy aroma and punchy bitterness reminiscent of the Robusta cargo that shaped Cape Town’s taste in coffee.</t>
+  </si>
+  <si>
+    <t>This blend brings you Cape Town’s taste in coffee. With South Africa as a stopping point on the old trade routes, Asian coffees shaped local taste over time. World Explorations Cape Town Lungo reflects this preference with a blend of Indian Arabica and Robusta. It results in our most intense Lungo – full-bodied and with a punchy bitter note and woodsy aroma. Enjoy it like a local: Add a splash of milk to your long cup and experience the silky texture.</t>
+  </si>
+  <si>
+    <t>Lungo 110ml</t>
+  </si>
+  <si>
+    <t>Roasted, Woody</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441093136414/capetown-envivo-lungo-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/cape-town-envivo-lungo_L.png</t>
+  </si>
+  <si>
+    <t>Roasted with a peppery note</t>
+  </si>
+  <si>
+    <t>Walk the streets of Miami and you’ll pass dozens of ventanitas. These ‘little windows’ are portholes to Cuba; miniature coffee shops dishing out small bites and coffee—the short Cafecito or the larger Colado to share. The city is a melting pot of traditions and World Explorations Miami Espresso is a bold blend of Arabica and Robusta coffees that echoes that. Caribbean Arabica joins Latin American coffees, sealing the authenticity of this archetypal Cuban-style cup. While Americans grab their tall coffees to-go, Miami reflects its strong Hispanic influence: coffee is short and shared.</t>
+  </si>
+  <si>
+    <t>Short, dark split roasting and a fine grind help evoke every ventanita’s Cuban Cafecito. Always sweetened with a sprinkle of brown sugar, this coffee is as vibrant as the context in which it’s enjoyed. While Americans grab their tall coffees to-go, Miami reflects its strong Hispanic influence: coffee is short and shared. Intense, with thick crema, its strong roasted character begs for brown sugar to soften the bitter notes. Enjoy your Cafecito with brown sugar and people because in Miami, coffee is a way to be together.</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15104178651166/before-PLP-318x318px.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15143388676126/AT-B2C-2022-WEX-Miami-Image-Set-Desktop.png</t>
+  </si>
+  <si>
+    <t>Cereal &amp; Spicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embodying the spirit of this lively and colourful city, World Explorations Rio de Janeiro Espresso reflects the country’s deeply rooted heritage of both growing and drinking coffee. An intense, exotic and velvety espresso crafted exclusively with Brazilian Arabicas. Its unique touch of sandalwood and herbal notes will give you a glimpse into the Brazilian way of life. Drink it like a local: Double your espresso with hot water to taste the typical smooth Carioca coffee.
+</t>
+  </si>
+  <si>
+    <t>An Arabica-only espresso with a complex split roast delivers a surprisingly full body and strong roasted notes graced with exotic herbal aromas</t>
+  </si>
+  <si>
+    <t>Spicy</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/B2C-enriched-pdp-wex-2022/istanbul-espresso/main-image_S.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15414727049246/before-PLP-318x318px.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15200754532382/C-0889-Responsive-PDP-Main-6272x2432.jpg?impolicy=productPdpSafeZone&amp;imwidth=1238</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15430408437790/C-0888-before-PLP-318x318px.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Roasted with a fruity note and a hint of almond</t>
+  </si>
+  <si>
+    <t>Istanbul Espresso takes you back in time to the original coffeehouses. This intense ambrosial brew bursts with boldness, wild ripe fruits, and a delicate almond touch. Thick and velvety in homage to Turkish coffee, its Ethiopian Arabica and Indian Robusta remind us of this city at the crossroads of the ancient coffee trade routes. It’s a blend as cosmopolitan as the crowd gathered in an Istanbul coffeehouse. Enjoy it like a local: Accompany it with a glass of water and a piece of Turkish Delight.</t>
+  </si>
+  <si>
+    <t>A complex espresso full of wild aromatics and a balance of both bitter roasted and fruity notes, with a touch of acidity and an almond finish that hints at sweetness.</t>
+  </si>
+  <si>
+    <t>Fruity, Roasted</t>
+  </si>
+  <si>
+    <t>Rich &amp; Full-bodied</t>
+  </si>
+  <si>
+    <t>An intense all-Arabica coffee best enjoyed black to savour the pure taste beloved by Swedes – malty, with a hint of rich bitterness.</t>
+  </si>
+  <si>
+    <t>Swedes are among the world’s biggest coffee consumers. Wander around Stockholm, and you’ll often find intense black coffees with a malty savoury note coming from the distinctive Monsoon Arabica. World Explorations Stockholm Lungo recreates the aromatic profile of a Swedish coffee by coupling Monsooned Malabar with Colombian Arabica for an intense, sweet cup with a hint of bitterness. Drink it like a local: Share your large flavourful cup and cinnamon rolls with friends and family.</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15906838806558/stockholm-fortissio-lungo-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/13753029689374/C-0686-Main-PDP-Lungo-Stockholm-OL.jpg?impolicy=productPdpSafeZone&amp;imwidth=1238</t>
+  </si>
+  <si>
+    <t>Cereal and biscuity, with a hint of citrus</t>
+  </si>
+  <si>
+    <t>Travel the world through coffee – and discover unique and typical tastes brought to you from cities around the world</t>
+  </si>
+  <si>
+    <t>A balanced coffee with light bitterness, cereal biscuity notes, pleasant acidity and a hint of citrus.</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/B2C-enriched-pdp-wex-2022/paris-espresso/main-image_S.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15414968844318/C-0887-before-PLP-318x318px.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Floral &amp; Complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The high quality Arabicas deliver exceptional flowery aromas and complex tastes worthy of Tokyo’s refined palate.
+</t>
+  </si>
+  <si>
+    <t>Known for tea, the Japanese also have a real affinity for coffee. Striving for sophistication and natural sweetness, they love both a rich coffee and a balance of elegant aromas. World Explorations Tokyo Lungo captures the essence of these preferences with refined Ethiopian and Mexican Arabicas. Complex, floral, with a hint of acidity – you will be pleasantly surprised by this cup. Drink it like a local: Extract your long black cup up to 150ml and take time to savour its aromas.</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15942164447262/ol-tokyo-vivalto-lungo-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/tokyo-vivalto-lungo_S.png</t>
+  </si>
+  <si>
+    <t>Round &amp; Smooth</t>
+  </si>
+  <si>
+    <t>From coffeehouse to home coffee gathering, this balanced blend of smooth and silky South American Arabicas pairs perfectly with your viennoiserie.</t>
+  </si>
+  <si>
+    <t>Vienna’s coffeehouse tradition shaped the coffee culture of this vibrant city, known for its many recipes and the smoothness of its coffee. World Explorations Vienna Lungo recreates this balanced and pleasant Viennese taste by pairing sweet Brazilian and Colombian Arabicas, lightly roasted by our experts to enhance the malty and aromatic notes in the cup. Enjoy it like a local: Top up your Lungo with hot water for a 150ml cup and pair it with a slice of cake.</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441093333022/vienna-linizio-lungo-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/vienna-linizio-lungo_XL.png</t>
+  </si>
+  <si>
+    <t>Fruity with fine acidity</t>
+  </si>
+  <si>
+    <t>Venice has a long history of importing the world’s coffees and expertly roasting these diverse coffees into harmony. Their expertise inspired the beautifully balanced roast of Ispirazione Venezia. Worthy of a noble dessert, the classic caramel and cereal notes of this coffee marry elegantly with the decadent ingredients of this rich tiramisu.</t>
+  </si>
+  <si>
+    <t>WORLD EXPLORATIONS SHANGHAI LUNGO is an insight into the emerging Asian coffee culture. Crafted from Kenyan, Chinese and Indonesian Arabicas, this distinctive light-roast blend will please the palate with its berry notes and fine acidity. Enjoy it like a local: Lengthen this long cup of coffee with a splash of cream and take it on-the-go</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16106997547038/shanghai-lungo-plp.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/shangai-lungo_S.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/buenos-aires-lungo_L.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441093759006/buenos-aires-lungo-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Sweet &amp; Cereal</t>
+  </si>
+  <si>
+    <t>A destination for true foodies, Buenos Aires is a highlight of Argentina’s vibrant food scene. Sweetness prevails, and coffee is no exception: they love it sweet and milky!</t>
+  </si>
+  <si>
+    <t>WORLD EXPLORATIONS BUENOS AIRES LUNGO blends a gently roasted Colombian Arabica with Ugandan Robusta to deliver distinct cereal and sweet popcorn notes. A tribute to the city’s love for smooth long cups. Drink it like a local: Add a generous drop of milk and sugar at will to your Lungo for an extra treat.</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Ethiopea</t>
+  </si>
+  <si>
+    <t>Indonesia - Fairtrade</t>
+  </si>
+  <si>
+    <t>OL20</t>
+  </si>
+  <si>
+    <t>OL21</t>
+  </si>
+  <si>
+    <t>OL22</t>
+  </si>
+  <si>
+    <t>OL23</t>
+  </si>
+  <si>
+    <t>OL24</t>
+  </si>
+  <si>
+    <t>OL25</t>
+  </si>
+  <si>
+    <t>Origins</t>
+  </si>
+  <si>
+    <t>Robusta Monsson</t>
+  </si>
+  <si>
+    <t>Master Origins India with Robusta Monsoon gets its intense, woody, spicy aromatics from the monsooned Robusta blended into Indian Arabica.</t>
+  </si>
+  <si>
+    <t>Monsooning coffees is unique to India’s southwest coast. Months of monsoonal winds repeatedly swell and dry the beans. It mimics the journey it used to take when sailing to Europe. If you’re changing track, try this coffee as a Latte Macchiato. You’ll still catch the long-lasting wood and spice aromatics and all of Master Origins India with Robusta Monsoon’s intensity. This Arabica Robusta blend makes a great coffee with milk.</t>
+  </si>
+  <si>
+    <t>Espresso 40ml, Lungo 110ml</t>
+  </si>
+  <si>
+    <t>Intense, Spicy</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441091170334/india-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/india_L.png</t>
+  </si>
+  <si>
+    <t>Wet hulled Arabica</t>
+  </si>
+  <si>
+    <t>Master Origins Indonesia wet-hulled Arabica is a race against rain.</t>
+  </si>
+  <si>
+    <t>Sumatran farmers wet-hull their coffee because of the humid climate. They remove the parchment when the coffee is soft and moist because exposed beans dry faster. The method is unique to them and produces the classic Indonesian taste - velvety thick, wildly aromatic, notes of cured tobacco. Try Master Origins Indonesia wet-hulled Arabica with a dash of milk - nutty, woody and roasted notes emerge in this intense coffee with milk.</t>
+  </si>
+  <si>
+    <t>Espresso 40 ml, Lungo 110ml</t>
+  </si>
+  <si>
+    <t>Intense, Cereal, Woody</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441091596318/indonesia-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/indonesia_S.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/colombia_S.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441091694622/colombia-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Late Harvest Arabica</t>
+  </si>
+  <si>
+    <t>Master Origins Colombia with Late Harvest uses only high-grown, washed processed Colombian Arabica.</t>
+  </si>
+  <si>
+    <t>Can you taste the lively acidity and the burst of winey red fruit aromas? That comes from those coffee farmers who dared to wait longer before harvesting their crop. Like your coffee with milk? Master Origins Colombia with Late Harvest Arabica makes a delicate and creamy cappuccino. Sweet biscuit notes emerge when this Colombian coffee combines with milk froth.</t>
+  </si>
+  <si>
+    <t>Espresso 40ml. Lungo 110ml</t>
+  </si>
+  <si>
+    <t>High up in the Andes</t>
+  </si>
+  <si>
+    <t>We traveled across remote Peruvian regions in search of some of the finest organic Arabica beans. High up above 1000 meters, tucked into the slopes of the Andes, we found them. Blessed with the meticulous care of smallholder farmers, Peru Organic is an elegant, fruity coffee accented by a smooth toasted cereal note.</t>
+  </si>
+  <si>
+    <t>An elegant organic Arabica crafted by remote smallholder farmers in Peru’s remote Andes’ mountains, graced with smooth toasted cereal and fruit notes. After going to such great lengths to source the finest organic Peruvian coffee, it was only natural to take the same care in roasting this coffee. Peru Organic is a single origin coffee roasted in two parts to bring a nuanced complexity to the final cup. The two splits are lightly roasted and highlight the bright and smooth character of the blend while revealing the exotic fruity notes.</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15448290885662/7734.10-PLP-318x318.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/peru_S.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/nicaragua_S.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441091792926/nicaragua-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>With "Black-Honey" Processed Arabica</t>
+  </si>
+  <si>
+    <t>If Black Honey processing were the easy road to a nectarous coffee, they’d all do it. But only a few farmers dare. It’s a rare process because it calls for meticulous monitoring. Master Origins Nicaragua with ‘Black-Honey’ processed Arabica contains this coffee. It gives this Nicaraguan Arabica its smooth honeyed texture and sweet cereal notes.</t>
+  </si>
+  <si>
+    <t>With ''Black-Honey'' processed Arabica, Master Origins Nicaragua is a nectarous coffee. It has a satiny smooth texture and warming sweet cereal notes. Its distinct sweetness comes from the rare Black-Honey process. If you like it with milk froth, Master Origins Nicaragua with ‘Black-Honey’ processed Arabica makes a rich latte macchiato. As a coffee with milk, it’s balanced and has nutty, roasted notes that surface.</t>
+  </si>
+  <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/ethiopia_L.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14441091891230/ethiopia-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Ethiopia with Dry Processed Arabica</t>
+  </si>
+  <si>
+    <t>This is Ethiopian Arabica at its finest - decadently aromatic.</t>
+  </si>
+  <si>
+    <t>It has an orange blossom aroma, but the rich fruit jam notes come from the sun-dried coffee in Master Origins Ethiopia with dry processed Arabica. Continually hand-turning the coffee cherry to ensure even drying calls for great care. And Ethiopian farmers have used this method for longer than anyone else. If you like milk and coffee, try Master Origins Ethiopia with dry processed Arabica with milk froth to make a cappuccino. You’ll find all the delicate floral notes still smoothly dancing through this cup of coffee with milk.</t>
+  </si>
+  <si>
+    <t>Capriccio</t>
+  </si>
+  <si>
+    <t>Cosi</t>
+  </si>
+  <si>
+    <t>Volutto</t>
+  </si>
+  <si>
+    <t>Volutto Decaffeinato</t>
+  </si>
+  <si>
+    <t>OL26</t>
+  </si>
+  <si>
+    <t>OL27</t>
+  </si>
+  <si>
+    <t>OL28</t>
+  </si>
+  <si>
+    <t>OL29</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/commons/img/coffees/OL/composition/ol_coffee-sleeves_capriccio_16-9.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15762782748702/capriccio.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Rich &amp; Distinctive</t>
+  </si>
+  <si>
+    <t>Capriccio is the rich, unique espresso that is ready to astonish with its complex and balanced bouquet.</t>
+  </si>
+  <si>
+    <t>Its distinct cereal notes are characteristic of the Brazilian Arabica and touch of Robusta we use. But then Capriccio surprises you with a fine acidity that gleams through - that comes from the high-grown South American Arabicas and the light roast. Adding milk will bring out the biscuit and caramel notes - it highlights the coffee’s sweetness. You can really indulge with this in a Capriccio cappuccino or Latte Macchiato.</t>
+  </si>
+  <si>
+    <t>Balanced, Cereal</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/commons/img/coffees/OL/composition/ol_coffee-sleeves_cosi_16-9_2x.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15762785566750/cosi.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Mild &amp; Delicately roasted</t>
+  </si>
+  <si>
+    <t>Light roasting classic coffees keeps their distinguished aromatics alive. Cosi meets your palate with a smile.</t>
+  </si>
+  <si>
+    <t>It’s a blend of world-renowned Arabicas - from East Africa and Latin America. Kenya brings the jammy ripe, red fruit notes to Costa Rica’s rich, sweet cereal base. The light roast and coarse grind keeps this espresso mild and rounded without losing any of its soul. Cosi with milk takes on an indulgent silky texture and sweet biscuit notes.</t>
+  </si>
+  <si>
+    <t>Fruity, Cereal</t>
+  </si>
+  <si>
+    <t>The delicate and generous aromas of Brazilian and Colombian Arabicas strike graceful harmony in this approachable espresso.</t>
+  </si>
+  <si>
+    <t>Sweet &amp; Light</t>
+  </si>
+  <si>
+    <t>Volluto is sunny living. The natural Brazilian Arabica mellows out in its pre-shipment resting time. The medium roast softens the Brazil’s cereal notes and turns them to sweet biscuit. And the washed Arabica from Colombia brings delightful fresh red fruit notes to the blend. The medium roast and grind rounds out these flavors and creates a perfectly balanced espresso. Volluto comforts like the smell of fresh, oven-baked brioche does. This sweet and light espresso stays in full-bodied balance when you add milk.</t>
+  </si>
+  <si>
+    <t>Balanced, Fruity, Cereal</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/volluto_S.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15762784452638/volluto-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/commons/img/coffees/OL/composition/ol_coffee-sleeves_volluto-decaffeinato_16-9.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/15942161104926/volluto-decaffeinato-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Sweet and light. Delightfully balanced cereal and fruity notes. Volluto has an easy way about it.</t>
+  </si>
+  <si>
+    <t>And Volluto Decaffeinato is faithful to form - Brazilian and Colombian coffees are carefully composed and now gently decaffeinated - for very sunny living. We decaffeinate naturally to make sure the coffee beans’ quality and taste is protected as much as possible. And just as with Volluto, in a Volluto Decaffeinato with milk you’ll taste the irresistible charm of those easy sweet biscuit and caramel notes with a splash of lively fruit aromas.</t>
+  </si>
+  <si>
+    <t>Cereal, Fruity, Balanced</t>
+  </si>
+  <si>
+    <t>Corto</t>
+  </si>
+  <si>
+    <t>Scuro</t>
+  </si>
+  <si>
+    <t>Chiaro</t>
+  </si>
+  <si>
+    <t>Cocoa Truffle</t>
+  </si>
+  <si>
+    <t>Vanilla Éclair</t>
+  </si>
+  <si>
+    <t>Caramel Crème Brulle</t>
+  </si>
+  <si>
+    <t>OL30</t>
+  </si>
+  <si>
+    <t>OL31</t>
+  </si>
+  <si>
+    <t>OL32</t>
+  </si>
+  <si>
+    <t>OL33</t>
+  </si>
+  <si>
+    <t>OL34</t>
+  </si>
+  <si>
+    <t>OL35</t>
+  </si>
+  <si>
+    <t>Very spicy and slightly smoked</t>
+  </si>
+  <si>
+    <t>Inspired by the dark roasted tastes and thick textures created by the expert baristas of Spain, we selected a blend of African Arabicas and Robusta, and roasted them long and dark to create a powerful, full-bodied taste, which becomes smoother and creamier with a splash of milk.</t>
+  </si>
+  <si>
+    <t>For BARISTA CREATIONS Corto, we took our inspiration from the dark roasts and thick textures created by the expert baristas in Spain, that is why it is easily recognizable by its raw strength and intense, roasty character. Corto can punch through milk with its rich aftertaste, elegant bitterness, and a thick, textured body. With a dash of hot milk and milk froth crowning the cup, you’ll experience Corto in the traditional cortado recipe’s way.</t>
+  </si>
+  <si>
+    <t>Capuccino, Latte Macchiato</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/14438025363486/corto-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/corto_L.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/scuro_L.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16291413262366/scuro-OL-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>With balanced biscuit notes</t>
+  </si>
+  <si>
+    <t>Taking our inspiration from Melbourne baristas - the masters of robust, but perfectly balanced tastes.</t>
+  </si>
+  <si>
+    <t>Our BARISTA CREATIONS Scuro shows you how intense your coffee can get while still staying beautifully in balance with milk. It’s just roasty enough to push through milk, and its delicate sweetness tempers its intensity to make it a compelling intense Cappuccino or Latte Macchiato.</t>
+  </si>
+  <si>
+    <t>Roasted, Balanced</t>
+  </si>
+  <si>
+    <t>With notes of caramel and sweet biscuits</t>
+  </si>
+  <si>
+    <t>Inspired by the baristas of Brooklyn, who value the natural sweetness of coffee and apply a light roast to protect it.</t>
+  </si>
+  <si>
+    <t>BARISTA CREATIONS Chiaro has hardly a hint of roastiness, and almost no bitterness or acidity you can perceive. It’s all creamy caramel and sweet biscuit notes when you add milk. The baristas in Brooklyn inspired us in the way their light roast values the natural sweetness of coffee and lends a decadent smoothness to the cup when you add milk.</t>
+  </si>
+  <si>
+    <t>48 g</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16154719715358/chiaro-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxATEhUSEhIVEA8VFRcXFRUVFhAWERUPFRUYFhUVFhUYHSggGBolGxUVITEhJikrLi4uFx8zODMtNygtLisBCgoKDg0OGhAQGzciHSAvLS4tKzctLysvLS0tKystLS0tNy4tNystLS0tLSstLSstLy0tLS0tLS0tLS0tLSsrLf/AABEIAKgBLAMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABAUDBgcCAQj/xABKEAABAwICBQgFBwsACwAAAAABAAIDBBEFIQYSMUFREyIyYXGBkaEHcrHB0RQjM0JSYqIVJENTc4KSsrPh8CVjZIOEk8LD0uLx/8QAGAEBAAMBAAAAAAAAAAAAAAAAAAECAwT/xAAkEQEAAgIBAwQDAQAAAAAAAAAAAQIDETEEEyESFEFhIjJR8P/aAAwDAQACEQMRAD8A7iiIgIiICIiAiIgIiIML6loNs3O4NBPiRkO9fRMfsO/D8Vy7Ea2QV5YWML+UJa02cOdt5+rdud8gt2mGobFpz3ta54bkMi1ouc+vggvOUP2T+H4r5y33HfhPsK17lH5WjcfvOELGnuMhcPBQsWopZWkFtM1m8uY+V1rbRcxgHvKDbYKqN5Ia4EjaN47Qsy5noHXStq+RbC3kncpd5dYtgZ0NVoye4u2gbL7TZdMQEREBERAREQEREBERAREQEREBERAREQEREBERAREQEREBERAREQEReJpA1pcdjQSewC6DQafCXzYrUk2ZTRahGqG35ZzQ61iLcXHfmFtxw/frnvbH8FC0abaN0ryBJPI6VwyvY2az8LW+Ks3VsY2uHmgwfk7/AFhHYGrxNg7HtLXvc5p2giL/AMVnOKQfbHg74IMSgP6Qeaga7oJByc1XC4NLoZA1hsNbki24N9oB4fdW5LWZi2KrZUMsWTNEUpBHSbcxuPi4LZlIIiICIiAiIgIiICIiAiIgIiICIiAiIgIiICIiAiIgIiICIiAiIgKJiObdXaHbexS1Cqzd1upRKYR44ABs/wDih1EIKspNigTFUSrJqccV4EA61IkK8tRL5yQ7VsuGy60bTvGR7QtfCtcDf0m9h9x9gUwiVqiIrqiIiAiIgIiICIiAiIgIiICIiAiIgIiICIiAiIgIiICIiAiIgKBP9Ie72BT1Xz/SHu9gUSmHycquncp1QVVVD1RZHe7NfWOUd7817Y5BKBVjgZ57vV96qg5WWAnnu9X3hTHJK9REV1BERAREQEREBERAREQEREBERAREQEREBERAREQEREBERAREQFW1B+cPd7ArJVdV9Ie72BRZMPFSVT1LlbVRyVLUlUWRHuzWSNyjvOa9xlBLBVpo+fnHer7wqdrlb4E1zXlzgQ0tsCeNwpjlEthRRnVY3BeDVnqV1UxFB+VO/wAsnyl3FBORQOXdxXg1L/8ALILJFW/LH9S9txA7wEE9FAfiORsy53DWAue0jJadj+m2IwXIw4NYP0hkMrbcSIwNXvKDoCLhlT6RcTlybLHD1Rxs2dsmsqvEMVq5L8rVTON82ukcGavqg28kHe63FaaH6WeKL13sb7So1NpJQyZMqoXHhyjL+BN1+eopREbsl1D90ELOccntq65cLWvqsBt1uAufFB+kmuBFwbjiNi+r8yU1ZKw3jJidvLXFpPe03VrBpdikfRrZB62rJ/UB9iD9DItL9GGP1NXDKah4kcyQNDg1rSQWg5huW3qW6ICIiAiIgIiICIiAiIgIiICq6v6Q93sCtFVVf0h7vYFFkwxVKpqlXFUqatka0XcQ0cSQB4lUWV79q9xqprNI6NnSnYbfZJefBgKrJdO6QZNbJIewNHi4g+SaG+4Y5rTrOaXZ2uBfV4ZbeOfUrlkzXdEh3YVzzQrTH5TUmAxiIOY4t+c1nF7M7WsPq6x37F0MQMcLuaCRvIBPirwrL45eCspphuuO93xUeW43+xSh9N15Lio8lS4cFFlxCTg3wPxQT3SlePlBVRLiknBvgfiocuLzfdH7v91A2PlljdOtTnxao+3bsaz3hQZqqY7ZXeNvZZBuj60DabBV8+lFOzIyax4Mu4+Iy8StMnjvm4lx67k+ajtiBcABtNkSqNMHxOqnuibyTHBri0BttZzQSe+4J67qmDR/hK3ilweCXOobMQdfUfCNZzWscGgOFjcE652butY5tCI5L/JKtskn6qZpjkPGxNr+FutWiUNPaLbAB4IFlq6WSJ7o5WGORuTmuyI/t1rDdShlaUJXgFelA616FR8xUfth/IF0Zc89C4/N5/2w/ptXQ1CRERAREQEREBERARYK4nk32yOo6xFwb6p2ELkWN6Luqbk1tWLjoySumh/5biD5rO+WtJ1K9cc2jw6lX4/RwfTVMMR4OkYHeBN1rtb6UcJYSBM+Zw3RxSkdznANPiuT1Xo+qmD5t0Mw4AmJ57Gv5v4lS1mCVcQvJTysHHV1md72Xb5q1clLcSiaWjmHU670zRD6Gke/rle1nfZgffyWt4h6Ua2RxcxkMN+DXPd4uNvJc/gfrmzAZDwYC8+DVa02j1fJ0Kd4HF+qwfiIPklprHMlYmeITq3SzEZenVS/ulsY8IwFTSvLjrOJc7i4lzvErYaPQKsdm+WOIdWu827Mh5q7pfRzCLGaeWQ7w3UY33nzWM9Rjj5axhvPw0BzhvKxiVpNhzjwGZ8F2Cg0HoGZinDzxkL5PJxt5K7io44xZsbWN4Na0exUnqojiFowT8y49oy6aCqgn5F7WslbrFwLbRu5rzzrfVc5foqDgueY7Qtc0nxW4aO1vKQxOJzLQHes3mu8wVbBn7kzEozYfRETC5cFDnCmXUeVq6XOrpmKvnareVqrqhiCrmaoUyn1AVfOFCUKVRpCpMjSo0saCHNIq6pxFsR1jm6x1W3zJ3HqA4qfK1aZibtaaRx+1YDcGtyAUxCFnFpRXNAayofGwbGss0DwFz33Vxh2m73Wjrmiph/WarW1EXBzHNA1rcDn1rTrr7dSh0zSKh+Ux8k5wlqWR8pSTjbPBbXMRO8ltyDxHbfmwct7onPOEwTNJEkE0jWO3ga/KM7g64Wj15by0jW2AMjwxo4axsAOxIS+Ar2CrPDdE8RmtydJKQd7miNvbeQtW04f6J61+cssUA4DWld4DVHmiGy+hc/m037f/tsXQlQ6HaMsoInRtkdKXv13OcGtz1Q2wA2Dm8Sr5QkREQEREBERAREQYasfNv8AVd7Cub4viLaaB872ucxgBIbbWsXBuVyBvuulzDmnsPsXJdNx/o+p/ZX8CD7lydRG7VdOCdVsx0GnmHSZcvyR4StcwfxEavmtkhc1wDmkFpAILTkQcwQRtC4limENNJHVtPO5JnKgWF5XOYASANtnm9uDCc3Erreijr0VKf8AZ4v6YWOXHWsbq1x3tadSmx7Bxzv1m+9e4W5OXhvvPtKzU2xy5Z5dEcEbcvP4e9e4c3ALNSxXaVGY/VcCra1EK8zK8YwBfJ6YEdaxtqha6y0z+Zn/AIF37pb8XHq1fLWK7LWaU0YxAta9m0Ndfud/cFeMdlHKEjgqLA6y1Tq7ntI/eHOHkD4rhxzNbT6XdesWp5dPjrmkX2L66pbxCo4Jcke5dcdTZx9iFw+QcQoU5CrJFAqSeKn3X0j2/wBrCoIVbO9vEKtqbqulT3P0dj7WstVGNrgq+oxKPdcqumKiSOU9+0o7UQkVFY52zmjzVDVYbK5/zcb5S47GNc91znmGgnvU8vK3zQqjkaOXEZPOIv0XFga0N1SRYi5dvC1xTMzuVLxEQ0vDvR7isuym5Jv2pnMYP4bl34Vs9F6H321qirawb2xMLj3PeR/Kugflgjbrg8DFIT4hufmo09dUS5QxOe77Ut44m9ZB5x7m94W22TWMaw1kUFPhVMXOfNJa7rGQRa5fLK6wtln4ELoVBhVPAPmYY4uOoxrSe0gXKqcC0eFM6Sqmk+UVb286QgNayMZ8nG36rcu+yqJMXfUggvDQfqA2A7d5VbXiq1a7bi6uiH12+KyxStcLtIcOIIK12gp2hmqTn25jsRkPJu1mlwP+beKz7s/xftx/WyooeG1Rkab7QbZb+tTFrE7jbOY0IiKUCIiAiIgIvhK8OmaN6D24LlekNI6akmhZbXkic1tzYaxGWe5dLfXMC526a4IDtU5gHI2O429y5OqnU1n/AHw6en8xMOO1GFYnBFJDLTTOheGdHnhpjN2kOj1gBlYjfYbLBdc0Qd+Y0vEQRDwYAvvLVDdmpKL8Sw21hYbx0dbPiBxymxSkgEjVJAuLg2O8X3rnyZfXHDamP0yys97v5ivcBsSFjgOXe7+Yr5UOs5YWb1WOHSZlvH2r1W0d8wqp1RqkOHfxVpHiNxe2sOIIWmO1bV9Nmd62rb1VY6emOwqVWThjbb1G/KN8mNJPAXcf4WrBNhVbN0Y9W/1pHBvlmfJXiNRqkbV5nd501zE6i7itTkr+TnY/cxwJ7Ac/K66ZB6PpHfTVAbxEbbn+Jx9ynUno0wxpu+J1Q7jK9xae1jbNPgtMPTWj9kZeprrVUSNyyr7iFOI5XMaNVo6IGwNIuAOobO5eQVhManSYncbYpVAqAp8qrq4Zd6hKBO1V0wUqpbwO9R5gra0javmUOQKdMFEkV6qSm6I4cJ6yGNw1ma2s8HYWMBcQeo2t3ruwC5l6KMPdy0sxFmtYGNO4l7rm3YGea6cu3FH47cuSfLwYm/ZHgF6AA2ZL6i1UQcck1aeU/cI8Rb3rmdBx3hdA0wl1aV33i0ed/cuf4bk4jiubPPmG+GPEtjoHh1tzhsVzWVBFrha3AbELY3ODmtvtWVZ3Ew0tHmErBZwS4AWyB9qtVUYXqtfYbSD8Vbrrx/r5c1+RERXVEREHh77LC+QqQQvJjQQZHOUSS6tjAsbqMHegpXqiqcPYSSLtN93wOxbocNYdt15GEQ/ZJ7SVE1i3MJi0xw0F9FIOi4O7bj4rHrvHSYe0ZjyXR24dCP0be8X9qzMgYNjWjsACxt01J+msZ7w59R6xaNVj3m56LHnab52GSn/kSqlH0YiHGRzfY2/nZbqvhKrHS0+VvcW+GrQ6JfrZyeqNob5uvfyU+mwKkj2RBx4vLn37jl5K1cVjcFrXDSvEM7Zb25l4FQ1os1oaOAAA8FjfXu3BenALC8BaM2CXEZNyg1GJzfaspkgCgzgINV0jx6aGSOR7OWidzXkGzmkbLHZnc7eCnYVizag2hje7qOo11vG3mpk9MxwIIBB2ggEEdir6GgbTv1o283ey51e7O48VlfDW3lpXLaqxmZIOlDMP928jxAUGdzd4cO1rx7law48xvShkHqyvPkbKW3Sin3sqB3g/9axnpY/rTvz/ABp8rY+3sDisDqVzujHK/wBWKU+xq3xukUJ6MNS7sH/uszMTkd0KOpPW98TR/UKn2v2d/wCnPho9VuzFNIG7y/UjAHHnkHyVTPiMNOCTC6eYbBe0I63XAJ7l10x1TwRyUcIItcyPkdn90Bv8yrsP0FpWP5WW9RJe41+gD1M2eN1euCsKTmmX30dCd1IJpxZ8ri5rbWDYRZrABuBsT+8tpXwBCtojTKZ2+r45wGZNgq+tdLbmmy1TE6Spfte4jhuUiHpZpW2UvhDNRjDzXOPOe4XBIbbJueWdyqKlrW5G+e9WE2E1BAbJC2ojHRDw4PaNwbI0hwHbdeI9Fi7ZTVDPVlhc38bQfNcuXFe07h0Y70iNSshO0gOvt9qtaupAia4HgqNmik+wR1Nv+D98wVgNG6hzQwtnDeDn0jB4t1z5LLtZfPhr3MfjyjnSPkTrgB7xsaSQHE5WJANsjtst4wfEG1ELJWtLNYZtdbWaeGW3tWtYfoU0EOeGNI+8+Z3cXBrAf3Ctup4GsaGtFgPG/EldGDHekatLDNelp/GGRERbsRERAREQEREBERB8X1EQfF8IREHh4WIhEQYnhYHsKIgwvhJWF1C4oiD4MIcVkbgAO1EQZo9Hot4upcWFQt2NC+oglMiaNgAXtEQEREBERB8IC+ag4BEQfdUcF9REBERAREQEREBERB//2Q==</t>
+  </si>
+  <si>
+    <t>Cocoa Flavored</t>
+  </si>
+  <si>
+    <t>Dark and bitter cocoa flavour meets the malted cereal note of the base espresso in Barista Creations Cocoa Truffle.</t>
+  </si>
+  <si>
+    <t>It’s rich and reminiscent of dark chocolate truffles. The base espresso is a blend of the finest South American Arabicas – sweet Bourbon beans from Brazil in harmony with the washed Colombian beans. A split roast brings out the best in each to create an incredibly smooth and rounded espresso – a great match for that dark cocoa flavour. A distinct cocoa note with a touch of almond sweetness and a hint of vanilla – that’s how you’ll recognize a Barista Creations Cocoa Truffle cappuccino.</t>
+  </si>
+  <si>
+    <t>Ristretto 25ml, Espresso 40ml, Cappuccino and Latte Macchiato</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16283400470558/cocoa-truffle-capsule-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/cocoa-truffle_L.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/vanilla-eclair_XL.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16283622670366/vanilla-eclair-coffee-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Vanilla Flavoured</t>
+  </si>
+  <si>
+    <t>It’s in sweet harmony that Barista Creations Vanilla Éclair flavour blends into a round, smooth Latin American Arabica espresso.</t>
+  </si>
+  <si>
+    <t>The base blend of Brazilian and Colombian Arabicas is known for its smooth taste and malted cereal notes – a real classic roasted coffee aroma. Barista Creations Vanilla Éclair plays into that full flavour with its own richness. The vanilla flavour brings a velvety layer to the taste of this flavoured coffee. If you dare the decadence, try it as a cappuccino and taste sweet almond notes dancing through the creamy custard taste.</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/shared_res/agility/n-components/pdp/sku-main-info/coffee-sleeves/ol/caramel-creme-brulee_L.png</t>
+  </si>
+  <si>
+    <t>https://www.nespresso.com/ecom/medias/sys_master/public/16107325259806/caramel-creme-brulee-XL.png?impolicy=product&amp;imwidth=150</t>
+  </si>
+  <si>
+    <t>Caramel Flavoured</t>
+  </si>
+  <si>
+    <t>Go ahead and dream a little. We did. The warming flavour of caramel softens the roasted notes of our most rounded and smooth espresso.</t>
+  </si>
+  <si>
+    <t>Creamy notes of caramel, coconut and vanilla dance through Barista Creations Caramel Crème Brûlée. The base blend for this flavoured coffee consists of some of South America’s finest Arabicas. We blended Brazilian Bourbon beans with washed Colombian coffee and split roasted them to bring them into beautiful harmony. The roast really develops that smooth texture and rounded mouthfeel. It’s into that harmony that we add the caramel flavour to bring this treat to the next level. Try Barista Creations Caramel Crème Brûlée as a cappuccino – it’s exceptionally creamy and brings out those notes of vanilla and coconut.</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1081,6 +1931,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1364,8 +2215,8 @@
   <dimension ref="A1:AD36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R34" sqref="R34"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4606,12 +5457,3229 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC7E57-8E6B-41A5-85C4-6F1AE8873BA1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V30" sqref="V30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="22.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="28" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="G2" s="7">
+        <v>13</v>
+      </c>
+      <c r="H2" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="N2" s="7">
+        <v>1</v>
+      </c>
+      <c r="O2" s="7">
+        <v>5</v>
+      </c>
+      <c r="P2" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>5</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="7">
+        <v>10</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="G3" s="7">
+        <v>12</v>
+      </c>
+      <c r="H3" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="N3" s="7">
+        <v>1</v>
+      </c>
+      <c r="O3" s="7">
+        <v>5</v>
+      </c>
+      <c r="P3" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>5</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="7">
+        <v>10</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="G4" s="7">
+        <v>10</v>
+      </c>
+      <c r="H4" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="N4" s="7">
+        <v>3</v>
+      </c>
+      <c r="O4" s="7">
+        <v>4</v>
+      </c>
+      <c r="P4" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>4</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W4" s="7">
+        <v>10</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="G5" s="7">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="N5" s="7">
+        <v>3</v>
+      </c>
+      <c r="O5" s="7">
+        <v>4</v>
+      </c>
+      <c r="P5" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>4</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="W5" s="7">
+        <v>10</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="G6" s="7">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="N6" s="7">
+        <v>4</v>
+      </c>
+      <c r="O6" s="7">
+        <v>2</v>
+      </c>
+      <c r="P6" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>4</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W6" s="7">
+        <v>10</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="G7" s="7">
+        <v>9</v>
+      </c>
+      <c r="H7" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="N7" s="7">
+        <v>4</v>
+      </c>
+      <c r="O7" s="7">
+        <v>2</v>
+      </c>
+      <c r="P7" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>4</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="W7" s="7">
+        <v>10</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="G8" s="7">
+        <v>8</v>
+      </c>
+      <c r="H8" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="N8" s="7">
+        <v>1</v>
+      </c>
+      <c r="O8" s="7">
+        <v>3</v>
+      </c>
+      <c r="P8" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>4</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8" s="7">
+        <v>10</v>
+      </c>
+      <c r="X8" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y8" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="G9" s="7">
+        <v>8</v>
+      </c>
+      <c r="H9" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="N9" s="7">
+        <v>4</v>
+      </c>
+      <c r="O9" s="7">
+        <v>4</v>
+      </c>
+      <c r="P9" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>3</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W9" s="7">
+        <v>10</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="G10" s="7">
+        <v>6</v>
+      </c>
+      <c r="H10" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="N10" s="7">
+        <v>3</v>
+      </c>
+      <c r="O10" s="7">
+        <v>3</v>
+      </c>
+      <c r="P10" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>3</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W10" s="7">
+        <v>10</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="Z10" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="AA10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="G11" s="7">
+        <v>10</v>
+      </c>
+      <c r="H11" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="N11" s="7">
+        <v>1</v>
+      </c>
+      <c r="O11" s="7">
+        <v>4</v>
+      </c>
+      <c r="P11" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>4</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W11" s="7">
+        <v>10</v>
+      </c>
+      <c r="X11" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="Z11" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="AA11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB11" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="G12" s="7">
+        <v>9</v>
+      </c>
+      <c r="H12" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="N12" s="7">
+        <v>1</v>
+      </c>
+      <c r="O12" s="7">
+        <v>4</v>
+      </c>
+      <c r="P12" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>4</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W12" s="7">
+        <v>10</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="G13" s="7">
+        <v>9</v>
+      </c>
+      <c r="H13" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="N13" s="7">
+        <v>1</v>
+      </c>
+      <c r="O13" s="7">
+        <v>4</v>
+      </c>
+      <c r="P13" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>5</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W13" s="7">
+        <v>10</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="Y13" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="Z13" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="AA13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB13" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="G14" s="7">
+        <v>8</v>
+      </c>
+      <c r="H14" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="N14" s="7">
+        <v>4</v>
+      </c>
+      <c r="O14" s="7">
+        <v>3</v>
+      </c>
+      <c r="P14" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>3</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U14" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W14" s="7">
+        <v>10</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y14" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="Z14" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="AA14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB14" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="G15" s="7">
+        <v>8</v>
+      </c>
+      <c r="H15" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="N15" s="7">
+        <v>2</v>
+      </c>
+      <c r="O15" s="7">
+        <v>3</v>
+      </c>
+      <c r="P15" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>2</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W15" s="7">
+        <v>10</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="Z15" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="AA15" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB15" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="G16" s="7">
+        <v>6</v>
+      </c>
+      <c r="H16" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N16" s="7">
+        <v>2</v>
+      </c>
+      <c r="O16" s="7">
+        <v>3</v>
+      </c>
+      <c r="P16" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>3</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W16" s="7">
+        <v>10</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y16" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="Z16" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="AA16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB16" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="G17" s="7">
+        <v>6</v>
+      </c>
+      <c r="H17" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="N17" s="7">
+        <v>1</v>
+      </c>
+      <c r="O17" s="7">
+        <v>2</v>
+      </c>
+      <c r="P17" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>3</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W17" s="7">
+        <v>10</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="Y17" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="Z17" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="AA17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB17" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="G18" s="7">
+        <v>6</v>
+      </c>
+      <c r="H18" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N18" s="7">
+        <v>1</v>
+      </c>
+      <c r="O18" s="7">
+        <v>2</v>
+      </c>
+      <c r="P18" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>2</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W18" s="7">
+        <v>10</v>
+      </c>
+      <c r="X18" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="Y18" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="Z18" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="AA18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB18" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="G19" s="7">
+        <v>5</v>
+      </c>
+      <c r="H19" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N19" s="7">
+        <v>2</v>
+      </c>
+      <c r="O19" s="7">
+        <v>1</v>
+      </c>
+      <c r="P19" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>2</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W19" s="7">
+        <v>10</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y19" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="Z19" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="AA19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="G20" s="7">
+        <v>4</v>
+      </c>
+      <c r="H20" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N20" s="7">
+        <v>2</v>
+      </c>
+      <c r="O20" s="7">
+        <v>1</v>
+      </c>
+      <c r="P20" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>3</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W20" s="7">
+        <v>10</v>
+      </c>
+      <c r="X20" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y20" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Z20" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="AA20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB20" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="G21" s="7">
+        <v>11</v>
+      </c>
+      <c r="H21" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="N21" s="7">
+        <v>1</v>
+      </c>
+      <c r="O21" s="7">
+        <v>5</v>
+      </c>
+      <c r="P21" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>3</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W21" s="7">
+        <v>10</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="Y21" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="Z21" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="AA21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB21" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="G22" s="7">
+        <v>8</v>
+      </c>
+      <c r="H22" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="N22" s="7">
+        <v>2</v>
+      </c>
+      <c r="O22" s="7">
+        <v>3</v>
+      </c>
+      <c r="P22" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>3</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W22" s="7">
+        <v>10</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y22" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z22" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="AA22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB22" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="G23" s="7">
+        <v>6</v>
+      </c>
+      <c r="H23" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I23" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N23" s="7">
+        <v>4</v>
+      </c>
+      <c r="O23" s="7">
+        <v>3</v>
+      </c>
+      <c r="P23" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>2</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W23" s="7">
+        <v>10</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Z23" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="AA23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB23" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="G24" s="7">
+        <v>6</v>
+      </c>
+      <c r="H24" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N24" s="7">
+        <v>4</v>
+      </c>
+      <c r="O24" s="7">
+        <v>3</v>
+      </c>
+      <c r="P24" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>3</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U24" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W24" s="7">
+        <v>10</v>
+      </c>
+      <c r="X24" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="Y24" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="Z24" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="AA24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB24" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="G25" s="7">
+        <v>5</v>
+      </c>
+      <c r="H25" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I25" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="N25" s="7">
+        <v>2</v>
+      </c>
+      <c r="O25" s="7">
+        <v>2</v>
+      </c>
+      <c r="P25" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>1</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W25" s="7">
+        <v>10</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="Z25" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA25" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB25" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="G26" s="7">
+        <v>4</v>
+      </c>
+      <c r="H26" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I26" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N26" s="7">
+        <v>4</v>
+      </c>
+      <c r="O26" s="7">
+        <v>2</v>
+      </c>
+      <c r="P26" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>1</v>
+      </c>
+      <c r="R26" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W26" s="7">
+        <v>10</v>
+      </c>
+      <c r="X26" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y26" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="Z26" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB26" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="G27" s="7">
+        <v>5</v>
+      </c>
+      <c r="H27" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="N27" s="7">
+        <v>3</v>
+      </c>
+      <c r="O27" s="7">
+        <v>3</v>
+      </c>
+      <c r="P27" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>2</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W27" s="7">
+        <v>10</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="Z27" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="AA27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB27" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="G28" s="7">
+        <v>4</v>
+      </c>
+      <c r="H28" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I28" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="N28" s="7">
+        <v>3</v>
+      </c>
+      <c r="O28" s="7">
+        <v>2</v>
+      </c>
+      <c r="P28" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>2</v>
+      </c>
+      <c r="R28" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S28" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T28" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U28" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W28" s="7">
+        <v>10</v>
+      </c>
+      <c r="X28" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y28" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="Z28" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="AA28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB28" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="G29" s="7">
+        <v>4</v>
+      </c>
+      <c r="H29" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="N29" s="7">
+        <v>3</v>
+      </c>
+      <c r="O29" s="7">
+        <v>2</v>
+      </c>
+      <c r="P29" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>2</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T29" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W29" s="7">
+        <v>10</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y29" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="Z29" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="AA29" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB29" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="G30" s="7">
+        <v>4</v>
+      </c>
+      <c r="H30" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="N30" s="7">
+        <v>3</v>
+      </c>
+      <c r="O30" s="7">
+        <v>2</v>
+      </c>
+      <c r="P30" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>2</v>
+      </c>
+      <c r="R30" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="S30" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U30" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V30" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="W30" s="7">
+        <v>10</v>
+      </c>
+      <c r="X30" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y30" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="Z30" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="AA30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB30" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H31" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I31" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="R31" s="7">
+        <v>1</v>
+      </c>
+      <c r="S31" s="7">
+        <v>5</v>
+      </c>
+      <c r="T31" s="7">
+        <v>5</v>
+      </c>
+      <c r="U31" s="7">
+        <v>1</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W31" s="7">
+        <v>10</v>
+      </c>
+      <c r="X31" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="Y31" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="Z31" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="AA31" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB31" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H32" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I32" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="R32" s="7">
+        <v>3</v>
+      </c>
+      <c r="S32" s="7">
+        <v>3</v>
+      </c>
+      <c r="T32" s="7">
+        <v>2</v>
+      </c>
+      <c r="U32" s="7">
+        <v>3</v>
+      </c>
+      <c r="V32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W32" s="7">
+        <v>10</v>
+      </c>
+      <c r="X32" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y32" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="Z32" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="AA32" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB32" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H33" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I33" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="P33" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q33" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="R33" s="7">
+        <v>5</v>
+      </c>
+      <c r="S33" s="7">
+        <v>1</v>
+      </c>
+      <c r="T33" s="7">
+        <v>1</v>
+      </c>
+      <c r="U33" s="7">
+        <v>4</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W33" s="7">
+        <v>10</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="Y33" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="Z33" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="AA33" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB33" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H34" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I34" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="P34" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="R34" s="7">
+        <v>1</v>
+      </c>
+      <c r="S34" s="7">
+        <v>1</v>
+      </c>
+      <c r="T34" s="7">
+        <v>2</v>
+      </c>
+      <c r="U34" s="7">
+        <v>2</v>
+      </c>
+      <c r="V34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W34" s="7">
+        <v>10</v>
+      </c>
+      <c r="X34" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="Z34" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="AA34" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB34" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H35" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I35" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="P35" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q35" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="R35" s="7">
+        <v>1</v>
+      </c>
+      <c r="S35" s="7">
+        <v>1</v>
+      </c>
+      <c r="T35" s="7">
+        <v>2</v>
+      </c>
+      <c r="U35" s="7">
+        <v>2</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W35" s="7">
+        <v>10</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="Z35" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="AA35" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB35" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H36" s="8">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I36" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="P36" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="R36" s="7">
+        <v>1</v>
+      </c>
+      <c r="S36" s="7">
+        <v>1</v>
+      </c>
+      <c r="T36" s="7">
+        <v>2</v>
+      </c>
+      <c r="U36" s="7">
+        <v>2</v>
+      </c>
+      <c r="V36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W36" s="7">
+        <v>10</v>
+      </c>
+      <c r="X36" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y36" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="Z36" s="7" t="s">
+        <v>608</v>
+      </c>
+      <c r="AA36" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB36" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>